<commit_message>
edit readme, add report.txt
</commit_message>
<xml_diff>
--- a/src/data/reports/HI710.xlsx
+++ b/src/data/reports/HI710.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="417">
   <si>
     <t>Index</t>
   </si>
@@ -1955,9 +1955,6 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
       <c r="D5" t="s">
         <v>31</v>
       </c>
@@ -2299,9 +2296,6 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" t="s">
         <v>31</v>
       </c>
@@ -2565,9 +2559,6 @@
       </c>
       <c r="B12">
         <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>

</xml_diff>